<commit_message>
Modify ExcelReader.java to FileExcelReader. Use test data from excel file as DataProvider.
</commit_message>
<xml_diff>
--- a/src/test/resources/testData.xlsx
+++ b/src/test/resources/testData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>city</t>
   </si>
@@ -25,10 +25,13 @@
     <t>Dubai</t>
   </si>
   <si>
-    <t>xxx</t>
-  </si>
-  <si>
     <t>London</t>
+  </si>
+  <si>
+    <t>Jumeirah Beach Hotel</t>
+  </si>
+  <si>
+    <t>Grand Plaza Apartments</t>
   </si>
 </sst>
 </file>
@@ -378,7 +381,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -394,15 +397,15 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>